<commit_message>
fix: MENA bar chart
</commit_message>
<xml_diff>
--- a/wit/web_bubble_chart/travel_market_summary.xlsx
+++ b/wit/web_bubble_chart/travel_market_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/130fda80f0432a83/Files/000_Archive/TravelMarketViz/utilities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/130fda80f0432a83/TravelMarketViz/wit/web_bubble_chart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_61905BD133772EF7847BF89C4A7BC93DD8FADAC8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FDB49A8-7321-624C-AF23-844BD0CAD15C}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_61905BD133772EF7847BF89C4A7BC93DD8FADAC8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8726C65B-AA05-FA4A-8207-4BBA24833DA4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -60702,8 +60702,8 @@
   </sheetPr>
   <dimension ref="A1:F921"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H174" sqref="H174"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163:XFD201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -60711,7 +60711,7 @@
     <col min="1" max="1" width="12.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -79137,5 +79137,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>